<commit_message>
Added testcases for Glioma 51to62 and OSA01Bai
</commit_message>
<xml_diff>
--- a/InputFiles/TC51_Canine_Study_OSA01_FileFormat_bai.xlsx
+++ b/InputFiles/TC51_Canine_Study_OSA01_FileFormat_bai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\ICDC All tab fix\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7325D391-8D06-4AC9-BE0A-D1576EF3A06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F55EBA8-3524-42DA-972C-A382F43A66BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -60,11 +60,17 @@
     <t>StudyFilesTab</t>
   </si>
   <si>
+    <t>TC51_Canine_Study_OSA01_FileFormat_bai_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC51_Canine_Study_OSA01_FileFormat_bai_WebData.xlsx</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
 MATCH (c)&lt;--(samp:sample)
 MATCH (f:file)-[*]-&gt;(c)
-WHERE s.clinical_study_designation IN ['MGT01'] and f.file_format in ['bai']
+WHERE s.clinical_study_designation IN ['OSA01'] and f.file_format in ['bai']
 OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
 WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
 RETURN  coalesce(c.case_id, '') AS `Case ID` ,
@@ -85,7 +91,7 @@
   <si>
     <t xml:space="preserve">MATCH (p:program)&lt;--(s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (c)&lt;--(r:registration)
 MATCH (cf:file)-[*]-&gt;(c)
-WHERE s.clinical_study_designation IN ['MGT01'] and cf.file_format in ['bai']
+WHERE s.clinical_study_designation IN ['OSA01'] and cf.file_format in ['bai']
 OPTIONAL MATCH (cf:file)-[*]-&gt;(c)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
 OPTIONAL MATCH (sf:file)--&gt;(s)
@@ -102,7 +108,7 @@
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
 MATCH (r:registration)--&gt;(c)
 MATCH (f:file)-[*]-&gt;(c)
-WHERE s.clinical_study_designation IN ['MGT01'] and f.file_format in ['bai']
+WHERE s.clinical_study_designation IN ['OSA01'] and f.file_format in ['bai']
 WITH DISTINCT samp AS samp, c, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
@@ -124,7 +130,7 @@
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
 MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['MGT01']
+WHERE s.clinical_study_designation IN ['OSA01']
 MATCH (f)--&gt;(samp:sample)
 WHERE f.file_format in ['bai']
 WITH
@@ -159,7 +165,7 @@
 MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
 MATCH (samp:sample)--&gt;(c)
 MATCH (c)&lt;--(demo:demographic)
-WHERE s.clinical_study_designation IN ['MGT01'] and f.file_format in ['bai']
+WHERE s.clinical_study_designation IN ['OSA01'] and f.file_format in ['bai']
 WITH
         DISTINCT f, c, demo, diag, s,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
@@ -182,12 +188,6 @@
   coalesce(s.clinical_study_designation,'') AS `Study Code`
   order by 'File Name' asc
   limit 100</t>
-  </si>
-  <si>
-    <t>TC51_Canine_Study_OSA01_FileFormat_bai_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC51_Canine_Study_OSA01_FileFormat_bai_WebData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -605,16 +605,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
@@ -622,16 +622,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
@@ -639,16 +639,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
@@ -656,16 +656,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>